<commit_message>
added levelBuilder class to classdiagramm and refactored userstories
</commit_message>
<xml_diff>
--- a/Planung/User Stories.xlsx
+++ b/Planung/User Stories.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NanoNode-Nexus\NanoNode-Nexus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NanoNode-Nexus\NanoNode-Nexus\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A2C55E1-4CD1-411C-9ADB-444385F1F289}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0F1774-04A9-4BF4-9CC6-C438BA75A1B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" xr2:uid="{6E36DC40-5F18-4EBE-9BC3-7D855008A313}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
   <si>
     <t>Priority scale</t>
   </si>
@@ -84,36 +84,15 @@
     <t>Acceptance Criteria</t>
   </si>
   <si>
-    <t>Implementing classes for movable entities</t>
-  </si>
-  <si>
-    <t>Implementing classes for entities</t>
-  </si>
-  <si>
-    <t>Implementing classes for game-renderer</t>
-  </si>
-  <si>
-    <t>Implementing classes for stationary entities</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementing classes for the rest of the derived entity classes </t>
-  </si>
-  <si>
     <t>Implementing game class</t>
   </si>
   <si>
     <t>Implementing database schema for save states</t>
   </si>
   <si>
-    <t>Implementing class for saving gamestate in DB</t>
-  </si>
-  <si>
     <t>Implementing 1 aditional tower</t>
   </si>
   <si>
-    <t>Implementing class for Fog of War</t>
-  </si>
-  <si>
     <t>Implementing one static game field</t>
   </si>
   <si>
@@ -121,6 +100,45 @@
   </si>
   <si>
     <t>Implementing algorithm for pathfinding (A*)</t>
+  </si>
+  <si>
+    <t>Implementing game-renderer</t>
+  </si>
+  <si>
+    <t>Implementing movable entities</t>
+  </si>
+  <si>
+    <t>Implementing stationary entities</t>
+  </si>
+  <si>
+    <t>Implementing saving gamestate in DB</t>
+  </si>
+  <si>
+    <t>Implementing Fog of War</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>I want the enemies to target my base and not have them move random</t>
+  </si>
+  <si>
+    <t>neccessity for base game</t>
+  </si>
+  <si>
+    <t>to save my level progress</t>
+  </si>
+  <si>
+    <t>I want different towers to chose from</t>
+  </si>
+  <si>
+    <t>I want to have to play to see the enemy base, and not from the beginning</t>
+  </si>
+  <si>
+    <t>I want random generated game fields and not one static only</t>
+  </si>
+  <si>
+    <t>save format for game field, for random generation as well as static fields, or maybe self edited</t>
   </si>
 </sst>
 </file>
@@ -591,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7C2921-B808-43C3-9286-7C3D73229528}">
   <dimension ref="C1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E4:E16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -691,12 +709,18 @@
       </c>
       <c r="D4" s="5"/>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -708,29 +732,41 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="G5" s="5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" t="s">
-        <v>19</v>
+      <c r="E6" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="G6" s="5">
+        <v>3</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -738,16 +774,22 @@
     </row>
     <row r="7" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="G7" s="5">
+        <v>4</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -759,12 +801,18 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="G8" s="5">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -772,16 +820,22 @@
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="G9" s="5">
+        <v>6</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -789,50 +843,68 @@
     </row>
     <row r="10" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" t="s">
-        <v>24</v>
+      <c r="E10" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
+      <c r="G10" s="5">
+        <v>7</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13" ht="30" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" t="s">
-        <v>25</v>
+      <c r="E11" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
+      <c r="G11" s="5">
+        <v>8</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" t="s">
-        <v>26</v>
+      <c r="E12" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="G12" s="5">
+        <v>9</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -840,33 +912,45 @@
     </row>
     <row r="13" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" t="s">
-        <v>27</v>
+      <c r="E13" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="G13" s="5">
+        <v>10</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:13" ht="45" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D14" s="5"/>
-      <c r="E14" t="s">
-        <v>28</v>
+      <c r="E14" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
+      <c r="G14" s="5">
+        <v>11</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -874,15 +958,19 @@
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D15" s="5"/>
-      <c r="E15" t="s">
-        <v>29</v>
+      <c r="E15" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="5">
+        <v>12</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -890,13 +978,9 @@
       <c r="M15" s="6"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" t="s">
-        <v>30</v>
-      </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1160,10 +1244,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C37" xr:uid="{0C4E6ECF-68E6-4C69-84EC-B67BB79105BC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C14 C17:C37" xr:uid="{0C4E6ECF-68E6-4C69-84EC-B67BB79105BC}">
       <formula1>$D$1:$G$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D37" xr:uid="{CC98014D-015B-493D-AA10-1DCCCD92FE62}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D14 D17:D37" xr:uid="{CC98014D-015B-493D-AA10-1DCCCD92FE62}">
       <formula1>$D$2:$G$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1185,6 +1269,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <a xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572" xsi:nil="true"/>
+    <TaxCatchAll xmlns="b43d7674-e72d-422b-be95-e22e3af49d99" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101006B8247937E6F6047838B253C0692F937" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c4b8eaee6a81220e587889abe47f8d5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0ba74dc7-3b53-4713-bb67-9e6187bc4572" xmlns:ns3="b43d7674-e72d-422b-be95-e22e3af49d99" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="adbd04a2623e67f13a6436da20248267" ns2:_="" ns3:_="">
     <xsd:import namespace="0ba74dc7-3b53-4713-bb67-9e6187bc4572"/>
@@ -1369,18 +1465,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <a xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572" xsi:nil="true"/>
-    <TaxCatchAll xmlns="b43d7674-e72d-422b-be95-e22e3af49d99" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CD4954-40DF-4E1B-A417-8AC111E78ABB}">
   <ds:schemaRefs>
@@ -1390,6 +1474,17 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE5B2139-0411-4F93-927B-CEF9303A0586}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0ba74dc7-3b53-4713-bb67-9e6187bc4572"/>
+    <ds:schemaRef ds:uri="b43d7674-e72d-422b-be95-e22e3af49d99"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7B1011D-8939-4CDB-887E-5FE3CE1D8589}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1406,15 +1501,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE5B2139-0411-4F93-927B-CEF9303A0586}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0ba74dc7-3b53-4713-bb67-9e6187bc4572"/>
-    <ds:schemaRef ds:uri="b43d7674-e72d-422b-be95-e22e3af49d99"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added A Text Field for the killedRobots
</commit_message>
<xml_diff>
--- a/Planung/User Stories.xlsx
+++ b/Planung/User Stories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NanoNode-Nexus\NanoNode-Nexus\Planung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucab\OneDrive\Desktop\Schule\NanoNode-Nexus\Planung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0F1774-04A9-4BF4-9CC6-C438BA75A1B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2803D49-583C-4BA9-ACE5-175D2EA23779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20715" windowHeight="13275" xr2:uid="{6E36DC40-5F18-4EBE-9BC3-7D855008A313}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="14496" xr2:uid="{6E36DC40-5F18-4EBE-9BC3-7D855008A313}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>Priority scale</t>
   </si>
@@ -93,16 +93,10 @@
     <t>Implementing 1 aditional tower</t>
   </si>
   <si>
-    <t>Implementing one static game field</t>
-  </si>
-  <si>
     <t>Implementing an algorithm for random game field generation</t>
   </si>
   <si>
     <t>Implementing algorithm for pathfinding (A*)</t>
-  </si>
-  <si>
-    <t>Implementing game-renderer</t>
   </si>
   <si>
     <t>Implementing movable entities</t>
@@ -218,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -235,7 +229,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -291,8 +284,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}" name="Tabelle1" displayName="Tabelle1" ref="C3:M37" totalsRowShown="0" dataDxfId="11">
-  <autoFilter ref="C3:M37" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}" name="Tabelle1" displayName="Tabelle1" ref="C3:M35" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="C3:M35" xr:uid="{35383E86-7FBF-4BC5-A1FB-8B8878744FCB}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{25C8B47E-6BAC-4926-B248-911D3C771B26}" name="Priority" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{9CE9A60A-229A-4767-BF36-858767E4CC66}" name="BusinessValue" dataDxfId="9"/>
@@ -311,9 +304,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -351,7 +344,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -457,7 +450,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -599,7 +592,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -607,28 +600,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7C2921-B808-43C3-9286-7C3D73229528}">
-  <dimension ref="C1:M37"/>
+  <dimension ref="C1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="57.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="29.7109375" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1"/>
-    <col min="9" max="9" width="26.85546875" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.140625" customWidth="1"/>
-    <col min="13" max="13" width="43.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" customWidth="1"/>
+    <col min="5" max="5" width="57.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" customWidth="1"/>
+    <col min="9" max="9" width="26.88671875" customWidth="1"/>
+    <col min="10" max="10" width="25.109375" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.109375" customWidth="1"/>
+    <col min="13" max="13" width="43.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C1" s="8" t="s">
         <v>0</v>
       </c>
@@ -648,7 +641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
@@ -668,7 +661,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
@@ -703,284 +696,261 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-    </row>
-    <row r="5" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C5" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="3:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="5"/>
-      <c r="E6" s="10" t="s">
-        <v>24</v>
+      <c r="E6" t="s">
+        <v>25</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>31</v>
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C7" s="5" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="5"/>
-      <c r="E7" s="10" t="s">
-        <v>27</v>
+      <c r="E7" t="s">
+        <v>19</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="7"/>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C8" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="6"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C9" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="6"/>
     </row>
-    <row r="10" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C10" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="10" t="s">
-        <v>28</v>
+      <c r="E10" t="s">
+        <v>21</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="6"/>
     </row>
-    <row r="11" spans="3:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="C11" s="5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" s="5"/>
-      <c r="E11" s="10" t="s">
-        <v>21</v>
+      <c r="E11" t="s">
+        <v>27</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
       <c r="M11" s="6"/>
     </row>
-    <row r="12" spans="3:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="C12" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="5"/>
-      <c r="E12" s="10" t="s">
-        <v>29</v>
+      <c r="E12" t="s">
+        <v>22</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
       <c r="M12" s="6"/>
     </row>
-    <row r="13" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C13" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="10" t="s">
-        <v>22</v>
+      <c r="E13" t="s">
+        <v>35</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="I13" s="5"/>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="6"/>
     </row>
-    <row r="14" spans="3:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
-        <v>3</v>
-      </c>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C14" s="5"/>
       <c r="D14" s="5"/>
-      <c r="E14" s="10" t="s">
-        <v>23</v>
-      </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="5">
-        <v>11</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="6"/>
     </row>
-    <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
-        <v>3</v>
-      </c>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C15" s="5"/>
       <c r="D15" s="5"/>
-      <c r="E15" s="10" t="s">
-        <v>37</v>
-      </c>
       <c r="F15" s="5"/>
-      <c r="G15" s="5">
-        <v>12</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
       <c r="M15" s="6"/>
     </row>
-    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
-      <c r="E16" s="10"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -990,7 +960,7 @@
       <c r="L16" s="5"/>
       <c r="M16" s="6"/>
     </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="F17" s="5"/>
@@ -1002,7 +972,7 @@
       <c r="L17" s="5"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="F18" s="5"/>
@@ -1014,7 +984,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="6"/>
     </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="F19" s="5"/>
@@ -1024,9 +994,9 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="F20" s="5"/>
@@ -1036,9 +1006,9 @@
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
-      <c r="M20" s="6"/>
-    </row>
-    <row r="21" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="F21" s="5"/>
@@ -1050,7 +1020,7 @@
       <c r="L21" s="5"/>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="F22" s="5"/>
@@ -1062,7 +1032,7 @@
       <c r="L22" s="5"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="F23" s="5"/>
@@ -1074,7 +1044,7 @@
       <c r="L23" s="5"/>
       <c r="M23" s="5"/>
     </row>
-    <row r="24" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
       <c r="F24" s="5"/>
@@ -1086,7 +1056,7 @@
       <c r="L24" s="5"/>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="F25" s="5"/>
@@ -1098,7 +1068,7 @@
       <c r="L25" s="5"/>
       <c r="M25" s="5"/>
     </row>
-    <row r="26" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
       <c r="F26" s="5"/>
@@ -1110,7 +1080,7 @@
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
     </row>
-    <row r="27" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="F27" s="5"/>
@@ -1122,7 +1092,7 @@
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
     </row>
-    <row r="28" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="F28" s="5"/>
@@ -1134,7 +1104,7 @@
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
     </row>
-    <row r="29" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="F29" s="5"/>
@@ -1146,7 +1116,7 @@
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
     </row>
-    <row r="30" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
       <c r="F30" s="5"/>
@@ -1158,7 +1128,7 @@
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
     </row>
-    <row r="31" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="F31" s="5"/>
@@ -1170,7 +1140,7 @@
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
     </row>
-    <row r="32" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="F32" s="5"/>
@@ -1182,7 +1152,7 @@
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
     </row>
-    <row r="33" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="F33" s="5"/>
@@ -1194,7 +1164,7 @@
       <c r="L33" s="5"/>
       <c r="M33" s="5"/>
     </row>
-    <row r="34" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="F34" s="5"/>
@@ -1206,7 +1176,7 @@
       <c r="L34" s="5"/>
       <c r="M34" s="5"/>
     </row>
-    <row r="35" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="F35" s="5"/>
@@ -1218,36 +1188,12 @@
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
     </row>
-    <row r="36" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-    </row>
-    <row r="37" spans="3:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C14 C17:C37" xr:uid="{0C4E6ECF-68E6-4C69-84EC-B67BB79105BC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15:C35 C4:C12" xr:uid="{0C4E6ECF-68E6-4C69-84EC-B67BB79105BC}">
       <formula1>$D$1:$G$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D14 D17:D37" xr:uid="{CC98014D-015B-493D-AA10-1DCCCD92FE62}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D15:D35 D4:D12" xr:uid="{CC98014D-015B-493D-AA10-1DCCCD92FE62}">
       <formula1>$D$2:$G$2</formula1>
     </dataValidation>
   </dataValidations>
@@ -1260,15 +1206,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="0ba74dc7-3b53-4713-bb67-9e6187bc4572">
@@ -1278,6 +1215,15 @@
     <TaxCatchAll xmlns="b43d7674-e72d-422b-be95-e22e3af49d99" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1466,20 +1412,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CD4954-40DF-4E1B-A417-8AC111E78ABB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE5B2139-0411-4F93-927B-CEF9303A0586}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="0ba74dc7-3b53-4713-bb67-9e6187bc4572"/>
     <ds:schemaRef ds:uri="b43d7674-e72d-422b-be95-e22e3af49d99"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3CD4954-40DF-4E1B-A417-8AC111E78ABB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>